<commit_message>
add test case for abs
</commit_message>
<xml_diff>
--- a/abs_testcase.xlsx
+++ b/abs_testcase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1580" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="1580" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="one host" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t>module</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -347,6 +347,22 @@
   </si>
   <si>
     <t>network</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>add volume</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>two services in defference host</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -482,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -556,6 +572,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,11 +899,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
@@ -948,7 +967,7 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -965,7 +984,7 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B4" s="38"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
@@ -980,7 +999,7 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="b">
@@ -997,7 +1016,7 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="7" t="b">
         <v>0</v>
       </c>
@@ -1012,7 +1031,7 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B7" s="39"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1046,7 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="7" t="b">
@@ -1044,7 +1063,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B9" s="39"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="7" t="b">
         <v>0</v>
       </c>
@@ -1059,7 +1078,7 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B10" s="39"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1121,7 +1140,7 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="38" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1138,7 +1157,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="39"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="7" t="b">
         <v>0</v>
       </c>
@@ -1153,7 +1172,7 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B16" s="39"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1168,7 +1187,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B17" s="39"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
@@ -1183,7 +1202,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B18" s="39"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
@@ -1198,8 +1217,8 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B19" s="39"/>
-      <c r="C19" s="40" t="s">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="8"/>
@@ -1213,8 +1232,8 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B20" s="39"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1226,7 +1245,7 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B21" s="38"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1241,7 +1260,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -1255,7 +1274,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="13" t="s">
         <v>36</v>
       </c>
@@ -1267,7 +1286,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="13" t="s">
         <v>37</v>
       </c>
@@ -1295,7 +1314,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -1306,7 +1325,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="12" t="s">
         <v>41</v>
       </c>
@@ -1355,10 +1374,10 @@
       </c>
     </row>
     <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="36" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -1369,8 +1388,8 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42"/>
-      <c r="C35" s="36"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="18" t="s">
         <v>56</v>
       </c>
@@ -1379,8 +1398,8 @@
       </c>
     </row>
     <row r="36" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="42"/>
-      <c r="C36" s="35" t="s">
+      <c r="B36" s="43"/>
+      <c r="C36" s="36" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -1391,8 +1410,8 @@
       </c>
     </row>
     <row r="37" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="13" t="s">
         <v>63</v>
       </c>
@@ -1401,8 +1420,8 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="42"/>
-      <c r="C38" s="36"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="13" t="s">
         <v>65</v>
       </c>
@@ -1411,8 +1430,8 @@
       </c>
     </row>
     <row r="39" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="42"/>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="43"/>
+      <c r="C39" s="36" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="13" t="s">
@@ -1423,8 +1442,8 @@
       </c>
     </row>
     <row r="40" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="13" t="s">
         <v>68</v>
       </c>
@@ -1433,7 +1452,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="36" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="12"/>
@@ -1445,7 +1464,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="36"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="12"/>
       <c r="D42" s="13" t="s">
         <v>71</v>
@@ -1458,7 +1477,7 @@
       <c r="A43" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="44" t="s">
         <v>73</v>
       </c>
       <c r="C43" s="19"/>
@@ -1478,7 +1497,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="43"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="19" t="s">
         <v>76</v>
       </c>
@@ -1490,34 +1509,43 @@
       </c>
     </row>
     <row r="46" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B47" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="s">
+    <row r="48" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="I47" s="18" t="s">
+      <c r="C48" s="19"/>
+      <c r="I48" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="12"/>
-    </row>
     <row r="49" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="12"/>
+      <c r="B49" s="12"/>
     </row>
     <row r="50" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
     </row>
     <row r="51" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
+    </row>
+    <row r="52" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1541,14 +1569,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="21" style="14" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B5" s="33"/>
+      <c r="C5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="26" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" s="18" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B8" s="43"/>
+      <c r="C8" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="23" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="23" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B3:B5"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
abs test case modify
</commit_message>
<xml_diff>
--- a/abs_testcase.xlsx
+++ b/abs_testcase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracyho/Desktop/rancher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracyho/Desktop/rancher/rancher-test_case/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1580" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4800" yWindow="1580" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="one host" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>module</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -363,6 +363,26 @@
   </si>
   <si>
     <t>two services in defference host</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>switch host</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete the host that had volume</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reuse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use the dist which state is detached</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -498,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -580,6 +600,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -595,12 +630,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -615,12 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,11 +922,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
@@ -967,7 +990,7 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="41" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -984,7 +1007,7 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B4" s="39"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
@@ -999,7 +1022,7 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="b">
@@ -1016,7 +1039,7 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B6" s="40"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="7" t="b">
         <v>0</v>
       </c>
@@ -1031,7 +1054,7 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1046,7 +1069,7 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="7" t="b">
@@ -1063,7 +1086,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B9" s="40"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="7" t="b">
         <v>0</v>
       </c>
@@ -1078,7 +1101,7 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B10" s="40"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1163,7 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="41" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1157,7 +1180,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="40"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="7" t="b">
         <v>0</v>
       </c>
@@ -1172,7 +1195,7 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B16" s="40"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1187,7 +1210,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B17" s="40"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
@@ -1202,7 +1225,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B18" s="40"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
@@ -1217,8 +1240,8 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="44" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="8"/>
@@ -1232,8 +1255,8 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B20" s="40"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1245,7 +1268,7 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B21" s="39"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1260,7 +1283,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -1274,7 +1297,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="13" t="s">
         <v>36</v>
       </c>
@@ -1286,7 +1309,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="33"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="13" t="s">
         <v>37</v>
       </c>
@@ -1314,7 +1337,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="39" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -1325,7 +1348,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="12" t="s">
         <v>41</v>
       </c>
@@ -1374,10 +1397,10 @@
       </c>
     </row>
     <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="33" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -1388,8 +1411,8 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="43"/>
-      <c r="C35" s="37"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="18" t="s">
         <v>56</v>
       </c>
@@ -1398,8 +1421,8 @@
       </c>
     </row>
     <row r="36" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="36" t="s">
+      <c r="B36" s="34"/>
+      <c r="C36" s="33" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -1410,8 +1433,8 @@
       </c>
     </row>
     <row r="37" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="13" t="s">
         <v>63</v>
       </c>
@@ -1420,8 +1443,8 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="43"/>
-      <c r="C38" s="37"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="13" t="s">
         <v>65</v>
       </c>
@@ -1430,137 +1453,149 @@
       </c>
     </row>
     <row r="39" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="43"/>
-      <c r="C39" s="36" t="s">
+      <c r="B39" s="34"/>
+      <c r="C39" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="34"/>
+      <c r="C40" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D40" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="12"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I41" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="37"/>
+      <c r="B42" s="33" t="s">
+        <v>69</v>
+      </c>
       <c r="C42" s="12"/>
       <c r="D42" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I42" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+    <row r="43" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="35"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B44" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="I43" s="18" t="s">
+      <c r="C44" s="19"/>
+      <c r="I44" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+    <row r="45" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I45" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="44"/>
-      <c r="C45" s="19" t="s">
+    <row r="46" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="32"/>
+      <c r="C46" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I46" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J46" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="30"/>
-      <c r="C46" s="12" t="s">
+    <row r="47" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="30"/>
+      <c r="C47" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="I47" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+    <row r="48" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="19" t="s">
+    <row r="49" spans="2:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="I48" s="18" t="s">
+      <c r="C49" s="19"/>
+      <c r="I49" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
-    </row>
-    <row r="50" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="12"/>
-    </row>
-    <row r="51" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="12"/>
-    </row>
-    <row r="52" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="12"/>
+    </row>
+    <row r="51" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="12"/>
+    </row>
+    <row r="52" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
+    </row>
+    <row r="53" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C34:C35"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1569,13 +1604,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="15" customWidth="1"/>
@@ -1635,8 +1670,8 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1649,8 +1684,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
+    <row r="4" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
       <c r="C4" s="13" t="s">
         <v>36</v>
       </c>
@@ -1661,8 +1696,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
+    <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="38"/>
       <c r="C5" s="13" t="s">
         <v>37</v>
       </c>
@@ -1673,13 +1708,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="26" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="27"/>
     </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>51</v>
       </c>
@@ -1687,9 +1722,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="36" t="s">
+    <row r="8" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="33" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1699,9 +1734,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+    <row r="9" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="13" t="s">
         <v>83</v>
       </c>
@@ -1709,33 +1744,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:10" s="13" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="23" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="23" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B8:B9"/>

</xml_diff>

<commit_message>
add rdb test case
</commit_message>
<xml_diff>
--- a/abs_testcase.xlsx
+++ b/abs_testcase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>module</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -150,35 +150,111 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>cancel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rancher ABS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Debug Mode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not select</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>abs service not exit before</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>abs service  exit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>abs service  exit before</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VPC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>network</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>add volume</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>default value（none）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>“”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>driver options</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>requirement underterment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>state</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>inactive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not create yet</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleted from aliyun console</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">detached </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete all services that use this volume</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>pass</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>cancel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rancher ABS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Debug Mode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>not select</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>abs service not exit before</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>abs service  exit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>abs service  exit before</t>
+    <t>active</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>one service</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>two services</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -186,118 +262,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>fail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VPC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Classic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>network</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>add volume</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>default value（none）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>“”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>driver options</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>requirement underterment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>state</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>inactive</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>not create yet</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>deleted from aliyun console</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">detached </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete all services that use this volume</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>active</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>one service</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>two services</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>one of the services delete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>switch volume</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -326,19 +294,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">upgrade </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>switch path</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -606,6 +566,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -629,21 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,8 +885,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.25"/>
@@ -977,7 +937,7 @@
     </row>
     <row r="2" spans="1:10" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
@@ -990,7 +950,7 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="33" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1007,7 +967,7 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B4" s="42"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +982,7 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="b">
@@ -1039,7 +999,7 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B6" s="43"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="7" t="b">
         <v>0</v>
       </c>
@@ -1054,7 +1014,7 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B7" s="43"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1069,7 +1029,7 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="7" t="b">
@@ -1086,7 +1046,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="7" t="b">
         <v>0</v>
       </c>
@@ -1101,7 +1061,7 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B10" s="43"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1077,7 @@
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7" t="b">
         <v>1</v>
@@ -1150,7 +1110,7 @@
     <row r="13" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="17"/>
       <c r="C13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1163,7 +1123,7 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1180,7 +1140,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="43"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="7" t="b">
         <v>0</v>
       </c>
@@ -1195,7 +1155,7 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B16" s="43"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1210,7 +1170,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B17" s="43"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
@@ -1225,7 +1185,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
@@ -1240,8 +1200,8 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44" t="s">
+      <c r="B19" s="35"/>
+      <c r="C19" s="36" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="8"/>
@@ -1255,8 +1215,8 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B20" s="43"/>
-      <c r="C20" s="45"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1268,7 +1228,7 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B21" s="42"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1283,94 +1243,73 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="13" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="13" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="26" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
-        <v>43</v>
+      <c r="B27" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C29" s="27"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="10" customFormat="1" ht="24" x14ac:dyDescent="0.25">
@@ -1385,210 +1324,160 @@
         <v>23</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="39"/>
+      <c r="C36" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="39"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="39"/>
+      <c r="C39" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="39"/>
+      <c r="C40" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="D40" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
-      <c r="C36" s="33" t="s">
+    <row r="41" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="38" t="s">
         <v>61</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="34"/>
-      <c r="C39" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="34"/>
-      <c r="C40" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="s">
-        <v>69</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="12"/>
       <c r="D43" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C44" s="19"/>
-      <c r="I44" s="18" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="45" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
       <c r="C46" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="I46" s="18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="30"/>
       <c r="C47" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C49" s="19"/>
-      <c r="I49" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
     </row>
-    <row r="51" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
     </row>
-    <row r="53" spans="2:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="C19:C20"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="B34:B41"/>
@@ -1596,6 +1485,11 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1658,7 +1552,7 @@
     </row>
     <row r="2" spans="1:10" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
@@ -1671,88 +1565,88 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="38"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="33" t="s">
-        <v>61</v>
+      <c r="B8" s="39"/>
+      <c r="C8" s="38" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="13" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>